<commit_message>
bug fixes and restructured files
</commit_message>
<xml_diff>
--- a/Reference/Arduino Bluetooth Remote tbyte Format Legend.xlsx
+++ b/Reference/Arduino Bluetooth Remote tbyte Format Legend.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kraj4\Documents\Arduino\Arduino Codes\Arduino_Bluetooth_Remote\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C957A-DD98-43EA-ADA8-68A3C1DBF719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572C104F-3D1B-451B-9951-DB9856A49BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F48471E1-1408-48F2-9661-0D72CCE12635}"/>
   </bookViews>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Internal Arrays</t>
   </si>
   <si>
     <t>Element</t>
@@ -254,12 +251,18 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>inputStateArray and txArray</t>
+  </si>
+  <si>
+    <t>tbyte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +293,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -460,12 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,6 +480,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,44 +810,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01F72D8-F0FB-4E57-B90D-2565CB1513DA}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="17"/>
+      <c r="A1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="22"/>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="C2" s="21"/>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -844,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -861,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -878,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
         <v>2</v>
@@ -895,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -912,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
@@ -929,7 +945,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -946,7 +962,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
@@ -963,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="4">
         <v>7</v>
@@ -980,7 +996,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="7">
         <v>0</v>
@@ -997,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -1014,7 +1030,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="7">
         <v>2</v>
@@ -1031,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="7">
         <v>3</v>
@@ -1048,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="7">
         <v>4</v>
@@ -1065,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="7">
         <v>5</v>
@@ -1082,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="7">
         <v>6</v>
@@ -1099,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="7">
         <v>7</v>
@@ -1116,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -1133,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1150,7 +1166,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
@@ -1167,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -1184,7 +1200,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="4">
         <v>4</v>
@@ -1201,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="4">
         <v>5</v>
@@ -1218,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="4">
         <v>6</v>
@@ -1235,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="4">
         <v>7</v>
@@ -1252,7 +1268,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="7">
         <v>0</v>
@@ -1269,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -1286,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="7">
         <v>2</v>
@@ -1303,7 +1319,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="7">
         <v>3</v>
@@ -1320,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="7">
         <v>4</v>
@@ -1337,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="7">
         <v>5</v>
@@ -1354,7 +1370,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="7">
         <v>6</v>
@@ -1371,7 +1387,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="7">
         <v>7</v>
@@ -1388,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" s="4">
         <v>0</v>
@@ -1405,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
@@ -1422,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="4">
         <v>2</v>
@@ -1439,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="4">
         <v>3</v>
@@ -1448,7 +1464,7 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1459,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" s="4">
         <v>4</v>
@@ -1476,7 +1492,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" s="4">
         <v>5</v>
@@ -1493,7 +1509,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" s="4">
         <v>6</v>
@@ -1510,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" s="4">
         <v>7</v>
@@ -1527,7 +1543,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="7">
         <v>0</v>
@@ -1544,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -1561,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45" s="7">
         <v>2</v>
@@ -1578,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="7">
         <v>3</v>
@@ -1595,29 +1611,29 @@
         <v>0</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="7">
+        <v>4</v>
+      </c>
+      <c r="E47" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="20">
+        <v>9</v>
+      </c>
+      <c r="B48" s="20">
+        <v>0</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="7">
-        <v>4</v>
-      </c>
-      <c r="E47" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="22">
-        <v>9</v>
-      </c>
-      <c r="B48" s="22">
-        <v>0</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="19">
-        <v>5</v>
-      </c>
-      <c r="E48" s="19">
+      <c r="D48" s="17">
+        <v>5</v>
+      </c>
+      <c r="E48" s="17">
         <v>6</v>
       </c>
     </row>
@@ -1629,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="7">
         <v>6</v>
@@ -1639,11 +1655,11 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>